<commit_message>
Correzioni in xlsx (casi 4,5,28,36)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA_S.a.s/LeoLab/5.02023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA_S.a.s/LeoLab/5.02023/report-checklist.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="889">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4676,6 +4676,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.ea71f8dc31^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il campo purpose_of_use non è valorizzato,"status":403,"instance":"/jwt-mandatory-field-missing</t>
+  </si>
+  <si>
+    <t>Il campo action_id non è corretto,"status":403,"instance":"/jwt-mandatory-field-malformed</t>
   </si>
 </sst>
 </file>
@@ -5595,7 +5601,7 @@
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota 2" xfId="41" customBuiltin="1"/>
+    <cellStyle name="Nota 2" xfId="41"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Testo descrittivo" xfId="15" builtinId="53" customBuiltin="1"/>
@@ -8060,10 +8066,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F375" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="K35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -8470,7 +8476,9 @@
       <c r="E13" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="23">
+        <v>45177</v>
+      </c>
       <c r="G13" s="24" t="s">
         <v>868</v>
       </c>
@@ -8514,7 +8522,9 @@
       <c r="E14" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="23">
+        <v>45177</v>
+      </c>
       <c r="G14" s="24" t="s">
         <v>869</v>
       </c>
@@ -9260,7 +9270,9 @@
       <c r="M35" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N35" s="25"/>
+      <c r="N35" s="25" t="s">
+        <v>887</v>
+      </c>
       <c r="O35" s="25" t="s">
         <v>139</v>
       </c>
@@ -9550,7 +9562,9 @@
       <c r="M43" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N43" s="25"/>
+      <c r="N43" s="25" t="s">
+        <v>888</v>
+      </c>
       <c r="O43" s="25" t="s">
         <v>139</v>
       </c>
@@ -10102,7 +10116,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="135">
+    <row r="59" spans="1:20" ht="135.75" thickBot="1">
       <c r="A59" s="20">
         <v>52</v>
       </c>
@@ -10140,7 +10154,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="135">
+    <row r="60" spans="1:20" ht="135.75" thickBot="1">
       <c r="A60" s="20">
         <v>53</v>
       </c>
@@ -10482,7 +10496,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="120">
+    <row r="69" spans="1:20" ht="120.75" thickBot="1">
       <c r="A69" s="20">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Aggiornamento dopo correzione degli errori del 14/09/2023
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA_S.a.s/LeoLab/5.02023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA_S.a.s/LeoLab/5.02023/report-checklist.xlsx
@@ -4621,67 +4621,67 @@
     <t>L'INOLTRO DEL REFERTO VA RIPETUTO. SE L'ERRORE PERSISTE E' GESTITO IN BACKOFFICE. I REFERTI RESTANO IN ATTESA DI ESSERE REINOLTRATI DOPO LA RISOLUZIONE DEL PROBLEMA</t>
   </si>
   <si>
-    <t>2023-09-08T16:40:00Z</t>
-  </si>
-  <si>
-    <t>2023-09-08T16:50:00Z</t>
-  </si>
-  <si>
     <t>2023-09-08T16:53:00Z</t>
   </si>
   <si>
     <t>2023-09-08T16:54:00Z</t>
   </si>
   <si>
-    <t>2023-09-08T16:51:00Z</t>
-  </si>
-  <si>
-    <t>463d591c8434257b</t>
-  </si>
-  <si>
-    <t>fc751d99227eb4f5</t>
-  </si>
-  <si>
-    <t>759b5f3a7783abc9</t>
-  </si>
-  <si>
-    <t>8922ca3316dfbd02</t>
-  </si>
-  <si>
-    <t>60adf2bcd597f6d9</t>
-  </si>
-  <si>
     <t>b76f7372276bf5f6</t>
   </si>
   <si>
     <t>3bbbc142483c8e79</t>
   </si>
   <si>
-    <t>74b094995d0cb124</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.94b93086c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.4c5853f9a64f23a03bf360edc86df254726bc41ba341ddec47620952e39c9a78.046bd5ef92^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.1cfbce3e2ea6115e39532217a87595250844292a296d1c58e76015a325319cf2.4b3f070d21^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.ce713098852728e51b4027718515a41fff939a84a2780e9b0e325107a085608e.b717652932^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.321b656d42050687f9398488c35ef14fae0109b9e7031750ad606e93f19eb22a.2745b3e71b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.ea71f8dc31^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il campo purpose_of_use non è valorizzato,"status":403,"instance":"/jwt-mandatory-field-missing</t>
   </si>
   <si>
     <t>Il campo action_id non è corretto,"status":403,"instance":"/jwt-mandatory-field-malformed</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.0ac7414303^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>449bcd754709bddf</t>
+  </si>
+  <si>
+    <t>2023-09-28T19:29:00Z</t>
+  </si>
+  <si>
+    <t>7c6641f578ee5ef4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.4c5853f9a64f23a03bf360edc86df254726bc41ba341ddec47620952e39c9a78.077b3da6ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceIde:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-09-28T19:30:00Z</t>
+  </si>
+  <si>
+    <t>398dd4059d0b8fc3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.1cfbce3e2ea6115e39532217a87595250844292a296d1c58e76015a325319cf2.ea051b5e04^^^^urn:ihe:iti:xdw:2013:workflowInstanceIde:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>62cfb2d648d5bdbc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.ce713098852728e51b4027718515a41fff939a84a2780e9b0e325107a085608e.962ea617b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.321b656d42050687f9398488c35ef14fae0109b9e7031750ad606e93f19eb22a.05eb4eb1e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f11e2b943674aafb</t>
+  </si>
+  <si>
+    <t>2023-09-28T19:28:00Z</t>
+  </si>
+  <si>
+    <t>b4d023079509eb27</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.f768065144^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -8066,10 +8066,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="K35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I375" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N51" sqref="N51"/>
+      <selection pane="bottomRight" activeCell="I383" sqref="I383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -8339,16 +8339,16 @@
         <v>47</v>
       </c>
       <c r="F10" s="23">
-        <v>45177</v>
+        <v>45197</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>139</v>
@@ -8385,16 +8385,16 @@
         <v>50</v>
       </c>
       <c r="F11" s="23">
-        <v>45177</v>
+        <v>45197</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>139</v>
@@ -8431,16 +8431,16 @@
         <v>52</v>
       </c>
       <c r="F12" s="23">
-        <v>45177</v>
+        <v>45197</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>868</v>
+        <v>879</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>139</v>
@@ -8477,16 +8477,16 @@
         <v>54</v>
       </c>
       <c r="F13" s="23">
-        <v>45177</v>
+        <v>45197</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>868</v>
+        <v>879</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>876</v>
+        <v>882</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>139</v>
@@ -8523,16 +8523,16 @@
         <v>56</v>
       </c>
       <c r="F14" s="23">
-        <v>45177</v>
+        <v>45197</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>869</v>
+        <v>879</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>877</v>
+        <v>885</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>139</v>
@@ -9252,10 +9252,10 @@
         <v>45177</v>
       </c>
       <c r="G35" s="24" t="s">
+        <v>868</v>
+      </c>
+      <c r="H35" s="24" t="s">
         <v>870</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>878</v>
       </c>
       <c r="I35" s="24" t="s">
         <v>865</v>
@@ -9271,7 +9271,7 @@
         <v>139</v>
       </c>
       <c r="N35" s="25" t="s">
-        <v>887</v>
+        <v>872</v>
       </c>
       <c r="O35" s="25" t="s">
         <v>139</v>
@@ -9544,10 +9544,10 @@
         <v>45177</v>
       </c>
       <c r="G43" s="24" t="s">
+        <v>869</v>
+      </c>
+      <c r="H43" s="24" t="s">
         <v>871</v>
-      </c>
-      <c r="H43" s="24" t="s">
-        <v>879</v>
       </c>
       <c r="I43" s="24" t="s">
         <v>865</v>
@@ -9563,7 +9563,7 @@
         <v>139</v>
       </c>
       <c r="N43" s="25" t="s">
-        <v>888</v>
+        <v>873</v>
       </c>
       <c r="O43" s="25" t="s">
         <v>139</v>
@@ -20925,16 +20925,16 @@
         <v>778</v>
       </c>
       <c r="F375" s="23">
-        <v>45177</v>
+        <v>45197</v>
       </c>
       <c r="G375" s="24" t="s">
-        <v>872</v>
+        <v>886</v>
       </c>
       <c r="H375" s="24" t="s">
-        <v>880</v>
+        <v>887</v>
       </c>
       <c r="I375" s="24" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="J375" s="25" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
Accreditamento LeoLab Giotto Informatica S.a.s. Palermo, ripetizione invio con WII del 05 ottobre 2023
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA_S.a.s/LeoLab/5.02023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GIOTTOINFOR/GIOTTO_INFORMATICA_S.a.s/LeoLab/5.02023/report-checklist.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="892">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4639,49 +4639,58 @@
     <t>Il campo action_id non è corretto,"status":403,"instance":"/jwt-mandatory-field-malformed</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.0ac7414303^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>449bcd754709bddf</t>
-  </si>
-  <si>
-    <t>2023-09-28T19:29:00Z</t>
-  </si>
-  <si>
-    <t>7c6641f578ee5ef4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.4c5853f9a64f23a03bf360edc86df254726bc41ba341ddec47620952e39c9a78.077b3da6ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceIde:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-09-28T19:30:00Z</t>
-  </si>
-  <si>
-    <t>398dd4059d0b8fc3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.1cfbce3e2ea6115e39532217a87595250844292a296d1c58e76015a325319cf2.ea051b5e04^^^^urn:ihe:iti:xdw:2013:workflowInstanceIde:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>62cfb2d648d5bdbc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.ce713098852728e51b4027718515a41fff939a84a2780e9b0e325107a085608e.962ea617b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.321b656d42050687f9398488c35ef14fae0109b9e7031750ad606e93f19eb22a.05eb4eb1e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f11e2b943674aafb</t>
-  </si>
-  <si>
-    <t>2023-09-28T19:28:00Z</t>
-  </si>
-  <si>
-    <t>b4d023079509eb27</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.f768065144^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-10-05T19:34:00Z</t>
+  </si>
+  <si>
+    <t>2023-10-05T19:35:00Z</t>
+  </si>
+  <si>
+    <t>2023-10-05T19:36:00Z</t>
+  </si>
+  <si>
+    <t>2023-10-05T19:37:00Z</t>
+  </si>
+  <si>
+    <t>2023-10-05T19:38:00Z</t>
+  </si>
+  <si>
+    <t>2023-10-05T19:39:00Z</t>
+  </si>
+  <si>
+    <t>14f97bbf2ccd321b</t>
+  </si>
+  <si>
+    <t>df6a3d5baf478cb0</t>
+  </si>
+  <si>
+    <t>1335c3f0371d1a64</t>
+  </si>
+  <si>
+    <t>4eae84560cfecb70</t>
+  </si>
+  <si>
+    <t>833b51ed8aa17920</t>
+  </si>
+  <si>
+    <t>4638d42019ad4500</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.efbc6c241c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.4c5853f9a64f23a03bf360edc86df254726bc41ba341ddec47620952e39c9a78.62778db5b3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.1cfbce3e2ea6115e39532217a87595250844292a296d1c58e76015a325319cf2.cd143eb471^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.ce713098852728e51b4027718515a41fff939a84a2780e9b0e325107a085608e.a7289a7615^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.321b656d42050687f9398488c35ef14fae0109b9e7031750ad606e93f19eb22a.691fa0a475^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.4b790a2aef1ce79c7c8ad9c6a057651f1f920cdf717dca6b9c06b4a904b64fdb.cbf472bef0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -8066,10 +8075,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I375" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I383" sqref="I383"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -8339,16 +8348,16 @@
         <v>47</v>
       </c>
       <c r="F10" s="23">
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>875</v>
+        <v>885</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>874</v>
+        <v>886</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>139</v>
@@ -8385,16 +8394,16 @@
         <v>50</v>
       </c>
       <c r="F11" s="23">
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>878</v>
+        <v>887</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>139</v>
@@ -8431,16 +8440,16 @@
         <v>52</v>
       </c>
       <c r="F12" s="23">
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>881</v>
+        <v>888</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>139</v>
@@ -8477,16 +8486,16 @@
         <v>54</v>
       </c>
       <c r="F13" s="23">
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>882</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>883</v>
+        <v>889</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>139</v>
@@ -8523,16 +8532,16 @@
         <v>56</v>
       </c>
       <c r="F14" s="23">
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>884</v>
+        <v>890</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>139</v>
@@ -20925,16 +20934,16 @@
         <v>778</v>
       </c>
       <c r="F375" s="23">
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="G375" s="24" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="H375" s="24" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="I375" s="24" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="J375" s="25" t="s">
         <v>139</v>

</xml_diff>